<commit_message>
Results comments addressed (initial stage).. continue results and discussion
</commit_message>
<xml_diff>
--- a/data/02_data_extraction/data_extraction_setJMGS_checkedSD.xlsx
+++ b/data/02_data_extraction/data_extraction_setJMGS_checkedSD.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shreyadimri/Library/CloudStorage/Dropbox/GitHub_Repo/GNM_Analysis/data/02_data_extraction/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shreyadimri/Library/CloudStorage/Dropbox/GitHub_Repo/Green_Nest_Material/data/02_data_extraction/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE56799F-180D-FC45-B030-08EE8FC92458}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3237DFFE-663B-4740-AFF9-F7ADCDCEC361}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1440" yWindow="500" windowWidth="64900" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1440" yWindow="500" windowWidth="71720" windowHeight="23280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1369,8 +1369,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AX77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R22" zoomScale="137" workbookViewId="0">
-      <selection activeCell="AD36" sqref="AD36"/>
+    <sheetView tabSelected="1" topLeftCell="N1" zoomScale="137" workbookViewId="0">
+      <selection activeCell="AQ52" sqref="AQ52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8780,7 +8780,7 @@
         <v>46</v>
       </c>
       <c r="AO49" s="6" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
       <c r="AP49" s="6" t="s">
         <v>67</v>
@@ -8932,7 +8932,7 @@
         <v>46</v>
       </c>
       <c r="AO50" s="6" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
       <c r="AP50" s="6" t="s">
         <v>67</v>
@@ -9081,7 +9081,7 @@
         <v>46</v>
       </c>
       <c r="AO51" s="6" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
       <c r="AP51" s="6" t="s">
         <v>67</v>
@@ -9230,7 +9230,7 @@
         <v>46</v>
       </c>
       <c r="AO52" s="6" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
       <c r="AP52" s="6" t="s">
         <v>67</v>
@@ -9379,7 +9379,7 @@
         <v>46</v>
       </c>
       <c r="AO53" s="6" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
       <c r="AP53" s="6" t="s">
         <v>67</v>
@@ -9528,7 +9528,7 @@
         <v>46</v>
       </c>
       <c r="AO54" s="6" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
       <c r="AP54" s="6" t="s">
         <v>67</v>
@@ -9677,7 +9677,7 @@
         <v>46</v>
       </c>
       <c r="AO55" s="6" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
       <c r="AP55" s="6" t="s">
         <v>67</v>
@@ -9826,7 +9826,7 @@
         <v>46</v>
       </c>
       <c r="AO56" s="6" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
       <c r="AP56" s="6" t="s">
         <v>67</v>
@@ -9975,7 +9975,7 @@
         <v>46</v>
       </c>
       <c r="AO57" s="12" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
       <c r="AP57" s="12" t="s">
         <v>67</v>
@@ -10124,7 +10124,7 @@
         <v>46</v>
       </c>
       <c r="AO58" s="12" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
       <c r="AP58" s="12" t="s">
         <v>67</v>
@@ -10273,7 +10273,7 @@
         <v>46</v>
       </c>
       <c r="AO59" s="12" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
       <c r="AP59" s="12" t="s">
         <v>67</v>
@@ -10422,7 +10422,7 @@
         <v>46</v>
       </c>
       <c r="AO60" s="12" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
       <c r="AP60" s="12" t="s">
         <v>67</v>
@@ -10571,7 +10571,7 @@
         <v>46</v>
       </c>
       <c r="AO61" s="12" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
       <c r="AP61" s="12" t="s">
         <v>67</v>
@@ -10720,7 +10720,7 @@
         <v>46</v>
       </c>
       <c r="AO62" s="12" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
       <c r="AP62" s="12" t="s">
         <v>67</v>
@@ -10869,7 +10869,7 @@
         <v>46</v>
       </c>
       <c r="AO63" s="12" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
       <c r="AP63" s="12" t="s">
         <v>67</v>
@@ -11018,7 +11018,7 @@
         <v>46</v>
       </c>
       <c r="AO64" s="12" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
       <c r="AP64" s="12" t="s">
         <v>67</v>
@@ -11167,7 +11167,7 @@
         <v>46</v>
       </c>
       <c r="AO65" s="12" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
       <c r="AP65" s="12" t="s">
         <v>67</v>

</xml_diff>